<commit_message>
[DOC] GEN MCU sample update
</commit_message>
<xml_diff>
--- a/Femto Project sample management.xlsx
+++ b/Femto Project sample management.xlsx
@@ -16,70 +16,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="33">
   <si>
     <t>No</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ECO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>OK</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>UART</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Booster</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>R10=68K ( Vout=9.8V)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>교수님</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>불출</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Trans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>CTX210605-R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>CTX210609-R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -107,27 +107,71 @@
       </rPr>
       <t>-R</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>FAIL</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PCB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>B-type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>C-type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Wire</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤재성</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>+5V CON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-Pin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-Pin</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spare</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Pipette Proto-type Sample</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Pipette Transformer PCB V1.0 Sample</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma LF Generator MCU V1.0 Sample</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -137,12 +181,20 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="&quot;#&quot;00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -201,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -467,33 +519,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -505,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -519,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -558,49 +599,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -905,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I9"/>
+  <dimension ref="B2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="L22" sqref="K22:L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -917,15 +982,20 @@
     <col min="6" max="6" width="21.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:9">
+      <c r="B2" s="48" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="3" spans="2:9" ht="17.25" thickBot="1"/>
     <row r="4" spans="2:9" ht="17.25" thickBot="1">
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="5" spans="2:9" s="2" customFormat="1" ht="17.25" thickBot="1">
       <c r="B5" s="28" t="s">
@@ -937,19 +1007,19 @@
       <c r="D5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -975,7 +1045,7 @@
       <c r="H6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1001,7 +1071,7 @@
       <c r="H7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1027,7 +1097,7 @@
       <c r="H8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1050,10 +1120,10 @@
       <c r="G9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="9" t="s">
+      <c r="H9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="50" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1061,17 +1131,17 @@
   <mergeCells count="1">
     <mergeCell ref="E4:I4"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J13"/>
+  <dimension ref="B2:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1079,17 +1149,22 @@
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="48" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="3" spans="2:10" ht="17.25" thickBot="1"/>
     <row r="4" spans="2:10" ht="17.25" thickBot="1">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="34"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="2:10" ht="17.25" thickBot="1">
       <c r="B5" s="28" t="s">
@@ -1098,10 +1173,10 @@
       <c r="C5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="34" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="28" t="s">
@@ -1124,10 +1199,10 @@
       <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="40" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1147,7 +1222,7 @@
       <c r="D7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="36" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="20" t="s">
@@ -1170,7 +1245,7 @@
       <c r="D8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="20" t="s">
@@ -1193,7 +1268,7 @@
       <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="20" t="s">
@@ -1216,7 +1291,7 @@
       <c r="D10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="38" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="20" t="s">
@@ -1239,7 +1314,7 @@
       <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="38" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="20" t="s">
@@ -1262,7 +1337,7 @@
       <c r="D12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="38" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="20" t="s">
@@ -1279,13 +1354,13 @@
       <c r="B13" s="13">
         <v>8</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="41" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="39" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="22" t="s">
@@ -1302,50 +1377,69 @@
   <mergeCells count="1">
     <mergeCell ref="F4:J4"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E9"/>
+  <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" ht="17.25" thickBot="1"/>
-    <row r="5" spans="2:5" ht="17.25" thickBot="1">
-      <c r="B5" s="28" t="s">
+    <row r="2" spans="2:7">
+      <c r="B2" s="48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="17.25" thickBot="1"/>
+    <row r="5" spans="2:7" ht="17.25" thickBot="1">
+      <c r="B5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
+      <c r="E5" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="36"/>
-    </row>
-    <row r="7" spans="2:5">
+        <v>24</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7" s="7">
         <v>2</v>
       </c>
@@ -1353,9 +1447,15 @@
       <c r="D7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="37"/>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="36"/>
+    </row>
+    <row r="8" spans="2:7">
       <c r="B8" s="7">
         <v>3</v>
       </c>
@@ -1363,20 +1463,34 @@
       <c r="D8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="38"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="7">
-        <v>4</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="38"/>
+      <c r="E8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="37"/>
+    </row>
+    <row r="9" spans="2:7" ht="17.25" thickBot="1">
+      <c r="B9" s="13">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[DOC] sample management update - Pipette v1.0/JTAG/Trans v2.0
</commit_message>
<xml_diff>
--- a/Femto Project sample management.xlsx
+++ b/Femto Project sample management.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proto_type" sheetId="1" r:id="rId1"/>
-    <sheet name="Transformer" sheetId="2" r:id="rId2"/>
-    <sheet name="LF GEN MCU" sheetId="3" r:id="rId3"/>
+    <sheet name="Pipette" sheetId="4" r:id="rId2"/>
+    <sheet name="JTAG" sheetId="5" r:id="rId3"/>
+    <sheet name="Transformer" sheetId="2" r:id="rId4"/>
+    <sheet name="LF GEN MCU" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="47">
   <si>
     <t>No</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -47,10 +49,6 @@
   </si>
   <si>
     <t>R10=68K ( Vout=9.8V)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>교수님</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -171,6 +169,79 @@
   </si>
   <si>
     <t>Plasma LF Generator MCU V1.0 Sample</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Femto</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAIL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commant</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1차 수리 완료 및 전달 5/13</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3, 8V DC/DC 교체 후에도 이상 동작 - Tr 교체 필요</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Pipette Transformer PCB V2.0 Sample</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Pipette V1.0 Sample</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Pipette JTAG V1.0 Sample</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F/W 용</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB CON</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tantal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -239,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +320,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +603,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -575,7 +652,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -666,6 +742,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -970,60 +1067,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I9"/>
+  <dimension ref="B2:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="K22:L23"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="3" width="9" style="1"/>
     <col min="6" max="6" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2" s="48" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="17.25" thickBot="1"/>
-    <row r="4" spans="2:9" ht="17.25" thickBot="1">
-      <c r="E4" s="42" t="s">
+    <row r="2" spans="2:10">
+      <c r="B2" s="47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="17.25" thickBot="1"/>
+    <row r="4" spans="2:10" ht="17.25" thickBot="1">
+      <c r="E4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
-    </row>
-    <row r="5" spans="2:9" s="2" customFormat="1" ht="17.25" thickBot="1">
-      <c r="B5" s="28" t="s">
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="52"/>
+    </row>
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="17.25" thickBot="1">
+      <c r="B5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="33" t="s">
+      <c r="H5" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="I5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="J5" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -1031,15 +1132,15 @@
         <v>3</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="26" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -1048,8 +1149,11 @@
       <c r="I6" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="J6" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7" s="7">
         <v>2</v>
       </c>
@@ -1059,7 +1163,7 @@
       <c r="D7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="20" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -1074,18 +1178,19 @@
       <c r="I7" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:9">
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="2:10">
       <c r="B8" s="7">
         <v>3</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1100,18 +1205,21 @@
       <c r="I8" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="17.25" thickBot="1">
+      <c r="J8" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="17.25" thickBot="1">
       <c r="B9" s="13">
         <v>4</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="22" t="s">
+      <c r="D9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="15" t="s">
@@ -1123,8 +1231,11 @@
       <c r="H9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="50" t="s">
-        <v>4</v>
+      <c r="I9" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="49" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1138,10 +1249,347 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J13"/>
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="3" width="9" style="1"/>
+    <col min="6" max="6" width="49.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" s="47" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="17.25" thickBot="1"/>
+    <row r="4" spans="2:6" ht="17.25" thickBot="1">
+      <c r="E4" s="41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" s="2" customFormat="1" ht="17.25" thickBot="1">
+      <c r="B5" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="7">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="7">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="7">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="2:6" ht="17.25" thickBot="1">
+      <c r="B11" s="13">
+        <v>6</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="49"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E25" sqref="E25:E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="2" max="3" width="9" style="1"/>
+    <col min="6" max="6" width="8.375" customWidth="1"/>
+    <col min="10" max="10" width="49.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="17.25" thickBot="1"/>
+    <row r="4" spans="2:10" ht="17.25" thickBot="1">
+      <c r="E4" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="52"/>
+    </row>
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="17.25" thickBot="1">
+      <c r="B5" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="7">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="7">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="2:10" ht="17.25" thickBot="1">
+      <c r="B10" s="13">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E4:I4"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1150,44 +1598,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="48" t="s">
-        <v>31</v>
+      <c r="B2" s="47" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="17.25" thickBot="1"/>
     <row r="4" spans="2:10" ht="17.25" thickBot="1">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="52"/>
     </row>
     <row r="5" spans="2:10" ht="17.25" thickBot="1">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="31"/>
+      <c r="D5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="3">
@@ -1199,11 +1647,11 @@
       <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>19</v>
+      <c r="E6" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>3</v>
@@ -1222,11 +1670,11 @@
       <c r="D7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>20</v>
+      <c r="E7" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>3</v>
@@ -1245,11 +1693,11 @@
       <c r="D8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>19</v>
+      <c r="E8" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>4</v>
@@ -1268,11 +1716,11 @@
       <c r="D9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>20</v>
+      <c r="E9" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>3</v>
@@ -1291,11 +1739,11 @@
       <c r="D10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>20</v>
+      <c r="E10" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>3</v>
@@ -1314,11 +1762,11 @@
       <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>20</v>
+      <c r="E11" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>4</v>
@@ -1337,11 +1785,11 @@
       <c r="D12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>20</v>
+      <c r="E12" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>4</v>
@@ -1354,40 +1802,275 @@
       <c r="B13" s="13">
         <v>8</v>
       </c>
-      <c r="C13" s="41" t="s">
-        <v>17</v>
+      <c r="C13" s="40" t="s">
+        <v>16</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="17" spans="2:9" ht="17.25" thickBot="1">
+      <c r="B17" s="47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="17.25" thickBot="1">
+      <c r="E18" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
+    </row>
+    <row r="19" spans="2:9" ht="17.25" thickBot="1">
+      <c r="B19" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="7">
+        <v>2</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="7">
+        <v>3</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="7">
+        <v>4</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="7">
+        <v>5</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="7">
+        <v>6</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="7">
+        <v>7</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="7">
+        <v>8</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="7">
+        <v>9</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="7">
+        <v>10</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="F4:J4"/>
+    <mergeCell ref="E18:I18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1398,29 +2081,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="48" t="s">
-        <v>32</v>
+      <c r="B2" s="47" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="17.25" thickBot="1"/>
     <row r="5" spans="2:7" ht="17.25" thickBot="1">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>29</v>
+      <c r="D5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -1429,15 +2112,15 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="35"/>
+        <v>22</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="7">
@@ -1448,12 +2131,12 @@
         <v>4</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="36"/>
+        <v>22</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="7">
@@ -1464,12 +2147,12 @@
         <v>4</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="37"/>
+        <v>22</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="2:7" ht="17.25" thickBot="1">
       <c r="B9" s="13">
@@ -1480,13 +2163,13 @@
         <v>4</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="49" t="s">
-        <v>28</v>
+      <c r="G9" s="48" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>